<commit_message>
Versioned all Excel Files
</commit_message>
<xml_diff>
--- a/examples/testproject/datadriven/data/raw/TM59/000_test__rawTM59results.xlsx
+++ b/examples/testproject/datadriven/data/raw/TM59/000_test__rawTM59results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\engDev\git_mf\ipyrun\examples\testproject\05 Model Files\001_Holmsdale_blkA_TM59Overheating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABC47CF-A784-4CF2-B4AB-6669A13763CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CB87C-18DF-4DC4-B4A5-B25DAD260261}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="-12120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>